<commit_message>
Started to add eeprom editor to controller.
Use the second latest dated code for the controller for the most stable
</commit_message>
<xml_diff>
--- a/LCDPlan.xlsx
+++ b/LCDPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koyug\Documents\GitHub\ArduinoIrrigationController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961134DD-10D6-4108-9402-FEC4D3F1A1B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF97C851-C183-4993-9713-37451C9ABE04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="60">
   <si>
     <t>C = Closed</t>
   </si>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -693,6 +693,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,7 +1015,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,6 +1322,9 @@
       </c>
       <c r="P5" s="8" t="s">
         <v>46</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="Z5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
UpdateVersion, start to add remote setting of eeprom values to the up time
</commit_message>
<xml_diff>
--- a/LCDPlan.xlsx
+++ b/LCDPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koyug\Documents\GitHub\ArduinoIrrigationController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF97C851-C183-4993-9713-37451C9ABE04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DD3658-83DF-4502-B25A-6C48F11C353A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>J G</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{5B3D49A0-A372-46B4-B9C2-5F6E65C93EB7}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{5B3D49A0-A372-46B4-B9C2-5F6E65C93EB7}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{5DB86630-4A3E-42A5-93D1-BE3C801DF5FF}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{5DB86630-4A3E-42A5-93D1-BE3C801DF5FF}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{F22F98A1-1D21-469B-A6E8-3F7D13E5022F}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{F22F98A1-1D21-469B-A6E8-3F7D13E5022F}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{EB50E110-6FB1-40EC-9BED-9785481DFFBF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>J G:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AI6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="AA19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="AG19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -222,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="AA20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="AA26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -270,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="AA28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -299,7 +323,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="60">
   <si>
     <t>C = Closed</t>
   </si>
@@ -448,9 +472,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -463,9 +484,6 @@
     <t>w</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -479,13 +497,19 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +556,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -637,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -695,6 +725,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,12 +1043,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH25"/>
+  <dimension ref="A1:BH29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,804 +1056,689 @@
     <col min="27" max="64" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="30">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30">
+        <v>2</v>
+      </c>
+      <c r="D1" s="30">
+        <v>3</v>
+      </c>
+      <c r="E1" s="30">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30">
+        <v>5</v>
+      </c>
+      <c r="G1" s="30">
+        <v>6</v>
+      </c>
+      <c r="H1" s="30">
+        <v>7</v>
+      </c>
+      <c r="I1" s="30">
+        <v>8</v>
+      </c>
+      <c r="J1" s="30">
         <v>9</v>
       </c>
-      <c r="D1" s="4">
-        <v>0</v>
-      </c>
-      <c r="E1" s="4">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="K1" s="30">
+        <v>10</v>
+      </c>
+      <c r="L1" s="30">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="30">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="30">
+        <v>13</v>
+      </c>
+      <c r="O1" s="30">
+        <v>14</v>
+      </c>
+      <c r="P1" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4">
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4">
         <v>1</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K2" s="4">
         <v>2</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L2" s="4">
         <v>3</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M2" s="4">
         <v>4</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N2" s="4">
         <v>5</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O2" s="4">
         <v>6</v>
       </c>
-      <c r="P1" s="5">
-        <v>7</v>
-      </c>
-      <c r="R1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA1" s="21">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="21">
+      <c r="P2" s="5">
+        <v>7</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="21">
         <v>1</v>
       </c>
-      <c r="AC1" s="21">
+      <c r="AC2" s="21">
         <v>2</v>
       </c>
-      <c r="AD1" s="21">
+      <c r="AD2" s="21">
         <v>3</v>
       </c>
-      <c r="AE1" s="21">
+      <c r="AE2" s="21">
         <v>4</v>
       </c>
-      <c r="AF1" s="21">
+      <c r="AF2" s="21">
         <v>5</v>
       </c>
-      <c r="AG1" s="21">
+      <c r="AG2" s="21">
         <v>6</v>
       </c>
-      <c r="AH1" s="21">
-        <v>7</v>
-      </c>
-      <c r="AI1" s="21">
+      <c r="AH2" s="21">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="21">
         <v>8</v>
       </c>
-      <c r="AJ1" s="21">
+      <c r="AJ2" s="21">
         <v>9</v>
       </c>
-      <c r="AK1" s="21">
+      <c r="AK2" s="21">
         <v>10</v>
       </c>
-      <c r="AL1" s="21">
+      <c r="AL2" s="21">
         <v>11</v>
       </c>
-      <c r="AM1" s="21">
+      <c r="AM2" s="21">
         <v>12</v>
       </c>
-      <c r="AN1" s="21">
+      <c r="AN2" s="21">
         <v>13</v>
       </c>
-      <c r="AO1" s="21">
+      <c r="AO2" s="21">
         <v>14</v>
       </c>
-      <c r="AP1" s="21">
+      <c r="AP2" s="21">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+    <row r="3" spans="1:42" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R3" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="Z3" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="R3" t="s">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AL4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="5" spans="1:42" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="17" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R5" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="U5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z5" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA5" s="3">
         <v>1</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB5" s="4">
         <v>2</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC5" s="4">
         <v>3</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD5" s="4">
         <v>4</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE5" s="4">
         <v>5</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AF5" s="4">
         <v>6</v>
       </c>
-      <c r="AG4" s="4">
-        <v>7</v>
-      </c>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4" t="s">
+      <c r="AG5" s="4">
+        <v>7</v>
+      </c>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AO4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="5">
+      <c r="AO5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:42" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="12" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="R5" s="29" t="s">
+      <c r="R6" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z6" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="14" t="s">
+      <c r="AA6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AB5" s="15" t="s">
+      <c r="AB6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AC5" s="15" t="s">
+      <c r="AC6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AD5" s="15" t="s">
+      <c r="AD6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AE6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AF5" s="15" t="s">
+      <c r="AF6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AG5" s="15" t="s">
+      <c r="AG6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="15" t="s">
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AM5" s="7" t="s">
+      <c r="AM6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AN5" s="7" t="s">
+      <c r="AN6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AO5" s="7" t="s">
+      <c r="AO6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AP5" s="8" t="s">
+      <c r="AP6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="Z8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>1</v>
+      </c>
+      <c r="B9" s="26">
+        <v>2</v>
+      </c>
+      <c r="C9" s="26">
+        <v>3</v>
+      </c>
+      <c r="D9" s="26">
+        <v>4</v>
+      </c>
+      <c r="E9" s="26">
         <v>5</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="F9" s="26">
+        <v>6</v>
+      </c>
+      <c r="G9" s="26">
+        <v>7</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="N9" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="H11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="N11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="Z7" t="s">
-        <v>16</v>
+      <c r="G12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="26"/>
+      <c r="P12" s="27" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
-        <v>1</v>
-      </c>
-      <c r="B8" s="26">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z13" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="26">
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z14" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="26">
-        <v>4</v>
-      </c>
-      <c r="E8" s="26">
-        <v>5</v>
-      </c>
-      <c r="F8" s="26">
-        <v>6</v>
-      </c>
-      <c r="G8" s="26">
-        <v>7</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="27"/>
-      <c r="Z8" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="S9" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C15" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="N11" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="O11" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="N15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="24"/>
-      <c r="R13" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z13" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26">
-        <v>0</v>
-      </c>
-      <c r="K14" s="26">
-        <v>0</v>
-      </c>
-      <c r="L14" s="26">
-        <v>0</v>
-      </c>
-      <c r="M14" s="26">
-        <v>0</v>
-      </c>
-      <c r="N14" s="26">
-        <v>0</v>
-      </c>
-      <c r="O14" s="26"/>
-      <c r="P14" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="24"/>
-      <c r="Z15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AO15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP15" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26">
-        <v>0</v>
-      </c>
-      <c r="K16" s="26">
-        <v>0</v>
-      </c>
-      <c r="L16" s="26">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26">
-        <v>0</v>
-      </c>
-      <c r="N16" s="26">
-        <v>0</v>
-      </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL16" s="7"/>
-      <c r="AM16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AV16" s="9"/>
-      <c r="AX16" s="9"/>
     </row>
     <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -1837,38 +1754,43 @@
         <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="L17" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q17" s="28"/>
+        <v>8</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="24"/>
+      <c r="R17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z17" s="20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
@@ -1878,344 +1800,600 @@
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
+      <c r="H18" s="26" t="s">
+        <v>55</v>
+      </c>
       <c r="I18" s="26"/>
-      <c r="J18" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="26"/>
+      <c r="J18" s="26">
+        <v>0</v>
+      </c>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
       <c r="L18" s="26">
         <v>0</v>
       </c>
       <c r="M18" s="26">
         <v>0</v>
       </c>
-      <c r="N18" s="26" t="s">
-        <v>55</v>
+      <c r="N18" s="26">
+        <v>0</v>
       </c>
       <c r="O18" s="26"/>
       <c r="P18" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="Z20" s="20" t="s">
-        <v>18</v>
-      </c>
+    <row r="19" spans="1:60" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="24"/>
+      <c r="Z19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:60" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26">
+        <v>0</v>
+      </c>
+      <c r="K20" s="26">
+        <v>0</v>
+      </c>
+      <c r="L20" s="26">
+        <v>0</v>
+      </c>
+      <c r="M20" s="26">
+        <v>0</v>
+      </c>
+      <c r="N20" s="26">
+        <v>0</v>
+      </c>
+      <c r="O20" s="26"/>
+      <c r="P20" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="9"/>
+      <c r="AR20" s="9"/>
+      <c r="AS20" s="9"/>
+      <c r="AT20" s="9"/>
+      <c r="AV20" s="9"/>
+      <c r="AX20" s="9"/>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AL21" t="s">
-        <v>15</v>
-      </c>
+      <c r="A21" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="28"/>
     </row>
     <row r="22" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="Z22" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26">
+        <v>0</v>
+      </c>
+      <c r="M22" s="26">
+        <v>0</v>
+      </c>
+      <c r="N22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="O22" s="26"/>
+      <c r="P22" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="Z24" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AL25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="Z26" t="s">
         <v>13</v>
       </c>
-      <c r="AA22" s="18" t="s">
+      <c r="AA26" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AB26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AC26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AD22" s="1" t="s">
+      <c r="AD26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE22" s="1" t="s">
+      <c r="AE26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
-      <c r="AH22" s="1"/>
-      <c r="AI22" s="1"/>
-      <c r="AJ22" s="1"/>
-      <c r="AK22" s="1"/>
-      <c r="AL22" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN22" s="4" t="s">
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AO22" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP22" s="5">
+      <c r="AO26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="Z23" t="s">
+    <row r="27" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="Z27" t="s">
         <v>14</v>
       </c>
-      <c r="AA23" s="6" t="s">
+      <c r="AA27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AB23" s="7" t="s">
+      <c r="AB27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="7" t="s">
+      <c r="AC27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AD23" s="7" t="s">
+      <c r="AD27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AE23" s="7" t="s">
+      <c r="AE27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AF23" s="12" t="s">
+      <c r="AF27" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AG23" s="12" t="str">
+      <c r="AG27" s="12" t="str">
         <f>"'"</f>
         <v>'</v>
       </c>
-      <c r="AH23" s="7" t="s">
+      <c r="AH27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="7" t="s">
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AK23" s="7" t="s">
+      <c r="AK27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AL23" s="7" t="s">
+      <c r="AL27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AM23" s="7" t="s">
+      <c r="AM27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AN23" s="7" t="s">
+      <c r="AN27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AO23" s="7" t="s">
+      <c r="AO27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AP23" s="8" t="s">
+      <c r="AP27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AQ23" s="9"/>
-      <c r="AR23" s="9" t="s">
+      <c r="AQ27" s="9"/>
+      <c r="AR27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AS23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT23" s="9" t="s">
+      <c r="AS27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AV23" s="9" t="s">
+      <c r="AV27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AX23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AY23" t="s">
+      <c r="AX27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY27" t="s">
         <v>6</v>
       </c>
-      <c r="BA23">
-        <v>0</v>
-      </c>
-      <c r="BB23">
-        <v>0</v>
-      </c>
-      <c r="BC23" t="s">
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BC27" t="s">
         <v>9</v>
       </c>
-      <c r="BD23">
-        <v>0</v>
-      </c>
-      <c r="BE23">
-        <v>0</v>
-      </c>
-      <c r="BG23" t="s">
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <v>0</v>
+      </c>
+      <c r="BG27" t="s">
         <v>28</v>
       </c>
-      <c r="BH23" t="s">
+      <c r="BH27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AA24" s="10" t="s">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AA28" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AB24" s="10" t="s">
+      <c r="AB28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AC24" s="10" t="s">
+      <c r="AC28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AD24" s="10" t="s">
+      <c r="AD28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AE24" s="10" t="s">
+      <c r="AE28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AF24" s="11" t="s">
+      <c r="AF28" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AG24" s="11" t="str">
+      <c r="AG28" s="11" t="str">
         <f>"'"</f>
         <v>'</v>
       </c>
-      <c r="AH24" s="10" t="s">
+      <c r="AH28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AI24" s="10"/>
-      <c r="AJ24" s="10" t="s">
+      <c r="AI28" s="10"/>
+      <c r="AJ28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AK24" s="10" t="s">
+      <c r="AK28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AL24" s="10" t="s">
+      <c r="AL28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AM24" s="10" t="s">
+      <c r="AM28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AN24" s="10" t="s">
+      <c r="AN28" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AO24" s="10" t="s">
+      <c r="AO28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AP24" s="10" t="s">
+      <c r="AP28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AQ24" s="9"/>
-      <c r="AR24" s="9" t="s">
+      <c r="AQ28" s="9"/>
+      <c r="AR28" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AS24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT24" s="9" t="s">
+      <c r="AS28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AV24" s="9" t="s">
+      <c r="AV28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AX24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AY24" t="s">
+      <c r="AX28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY28" t="s">
         <v>6</v>
       </c>
-      <c r="BA24">
-        <v>0</v>
-      </c>
-      <c r="BB24">
-        <v>0</v>
-      </c>
-      <c r="BC24" t="s">
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>0</v>
+      </c>
+      <c r="BC28" t="s">
         <v>9</v>
       </c>
-      <c r="BD24">
-        <v>0</v>
-      </c>
-      <c r="BE24">
-        <v>0</v>
-      </c>
-      <c r="BG24" t="s">
+      <c r="BD28">
+        <v>0</v>
+      </c>
+      <c r="BE28">
+        <v>0</v>
+      </c>
+      <c r="BG28" t="s">
         <v>28</v>
       </c>
-      <c r="BH24" t="s">
+      <c r="BH28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AA25" s="10" t="s">
+    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AA29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AB25" s="10" t="s">
+      <c r="AB29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AC25" s="10" t="s">
+      <c r="AC29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AD25" s="10" t="s">
+      <c r="AD29" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AE25" s="10" t="s">
+      <c r="AE29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AF25" s="11" t="s">
+      <c r="AF29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AG25" s="11" t="str">
+      <c r="AG29" s="11" t="str">
         <f>"'"</f>
         <v>'</v>
       </c>
-      <c r="AH25" s="10" t="s">
+      <c r="AH29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AI25" s="10"/>
-      <c r="AJ25" s="10" t="s">
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AK25" s="10" t="s">
+      <c r="AK29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AL25" s="10" t="s">
+      <c r="AL29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AM25" s="10" t="s">
+      <c r="AM29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AN25" s="10" t="s">
+      <c r="AN29" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AO25" s="10" t="s">
+      <c r="AO29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AP25" s="10" t="s">
+      <c r="AP29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AQ25" s="9"/>
-      <c r="AR25" s="9" t="s">
+      <c r="AQ29" s="9"/>
+      <c r="AR29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AS25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT25" s="9" t="s">
+      <c r="AS29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT29" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AV25" s="9" t="s">
+      <c r="AV29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AX25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="AY25" t="s">
+      <c r="AX29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY29" t="s">
         <v>6</v>
       </c>
-      <c r="BA25">
-        <v>0</v>
-      </c>
-      <c r="BB25">
-        <v>0</v>
-      </c>
-      <c r="BC25" t="s">
+      <c r="BA29">
+        <v>0</v>
+      </c>
+      <c r="BB29">
+        <v>0</v>
+      </c>
+      <c r="BC29" t="s">
         <v>9</v>
       </c>
-      <c r="BD25">
-        <v>0</v>
-      </c>
-      <c r="BE25">
-        <v>0</v>
-      </c>
-      <c r="BG25" t="s">
+      <c r="BD29">
+        <v>0</v>
+      </c>
+      <c r="BE29">
+        <v>0</v>
+      </c>
+      <c r="BG29" t="s">
         <v>28</v>
       </c>
-      <c r="BH25" t="s">
+      <c r="BH29" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>